<commit_message>
Success! Finished setting up the template excel sheet and our file's functionality with it
</commit_message>
<xml_diff>
--- a/Email_Automator/templates.xlsx
+++ b/Email_Automator/templates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayaanmahimwala/PythonProjects/Email-Automator/EmailAutomator/Email_Automator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kushalvajrala/ProgrammingProjects/Summer2020/EmailAutomator/Email_Automator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD34041C-7F8A-9740-AD2A-8E9BE16D6B59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47E2150-17BE-9347-B068-DAA0B6E69022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{0F43074A-802E-714D-994D-9E4E54681285}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{0F43074A-802E-714D-994D-9E4E54681285}"/>
   </bookViews>
   <sheets>
     <sheet name="templates" sheetId="1" r:id="rId1"/>
@@ -59,14 +59,14 @@
     <t>Required Prompts</t>
   </si>
   <si>
-    <t>parentName,studentName</t>
+    <t>[parentName],[studentName]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -417,18 +417,18 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
     <col min="3" max="3" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="404" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="404">
       <c r="A2" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
tested functionality in jupyter notebook; finished email parsing, now beginning construction of excel sheet
</commit_message>
<xml_diff>
--- a/Email_Automator/templates.xlsx
+++ b/Email_Automator/templates.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayaanmahimwala/PythonProjects/Email-Automator/EmailAutomator/Email_Automator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kushalvajrala/ProgrammingProjects/Summer2020/EmailAutomator/Email_Automator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF9FF90-E4C8-FF4A-886A-F6779AB4FCBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32BE1C1-0CD2-534A-88E1-A5B689D29780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" xr2:uid="{0F43074A-802E-714D-994D-9E4E54681285}"/>
   </bookViews>
   <sheets>
-    <sheet name="templates" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="templates" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Template Name</t>
   </si>
@@ -73,13 +73,43 @@
   </si>
   <si>
     <t>[studentName], Join us at CodeNinjas for our Python Program!</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Child's Name</t>
+  </si>
+  <si>
+    <t>Child Age</t>
+  </si>
+  <si>
+    <t>Email Date</t>
+  </si>
+  <si>
+    <t>Email Sent</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Response Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -426,14 +456,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52E0002-A110-4B4C-9617-31832C568BC0}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A09A0E6-BE6E-AA48-A499-8DE6C3C7EE47}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
@@ -441,7 +530,7 @@
     <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="404" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="404">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -469,7 +558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="409.5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -487,16 +576,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52E0002-A110-4B4C-9617-31832C568BC0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Work with openpyxl to populate excel sheet
</commit_message>
<xml_diff>
--- a/Email_Automator/templates.xlsx
+++ b/Email_Automator/templates.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kushalvajrala/ProgrammingProjects/Summer2020/EmailAutomator/Email_Automator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayaanmahimwala/PythonProjects/Email-Automator/EmailAutomator/Email_Automator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32BE1C1-0CD2-534A-88E1-A5B689D29780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D31E9E5-488E-EA42-A0D6-F8751834FE4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" xr2:uid="{0F43074A-802E-714D-994D-9E4E54681285}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Customers" sheetId="2" r:id="rId1"/>
     <sheet name="templates" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Template Name</t>
   </si>
@@ -103,13 +103,16 @@
   </si>
   <si>
     <t>Response Date</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -457,55 +460,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52E0002-A110-4B4C-9617-31832C568BC0}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -522,7 +529,7 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
@@ -530,7 +537,7 @@
     <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="404">
+    <row r="2" spans="1:4" ht="404" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -558,7 +565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="409.5">
+    <row r="3" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Working multi message parsing into excel
</commit_message>
<xml_diff>
--- a/Email_Automator/templates.xlsx
+++ b/Email_Automator/templates.xlsx
@@ -1,130 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayaanmahimwala/PythonProjects/Email-Automator/EmailAutomator/Email_Automator/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CB0692-C128-2A40-928E-4A5E41804A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="18900" windowWidth="33600" xWindow="0" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="Customers" sheetId="1" r:id="rId1"/>
-    <sheet name="templates" sheetId="2" r:id="rId2"/>
+    <sheet name="Customers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="templates" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Email Date</t>
-  </si>
-  <si>
-    <t>Response</t>
-  </si>
-  <si>
-    <t>Response Date</t>
-  </si>
-  <si>
-    <t>Template Name</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Template Message</t>
-  </si>
-  <si>
-    <t>Required Prompts</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>[studentName], Join us at CodeNinjas!</t>
-  </si>
-  <si>
-    <t>Hi [parentName], 
-This is Mike from CodeNinjas Cypress. Thank you for expressing interest in our program. Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something. I am sure that [studentName] will have a blast with one of our programs!
-Regards,
-CodeNinja Cypress</t>
-  </si>
-  <si>
-    <t>[parentName],[studentName]</t>
-  </si>
-  <si>
-    <t>Python Program</t>
-  </si>
-  <si>
-    <t>[studentName], Join us at CodeNinjas for our Python Program!</t>
-  </si>
-  <si>
-    <t>Hi [parentName], 
-This is Mike from CodeNinjas Cypress. Thank you for expressing interest in our program. Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something. I am sure that [studentName] will have a blast with one of our programs, especially our python program. We think it would be perfect for [studentName]
-Regards,
-CodeNinja Cypress</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Primary Email</t>
-  </si>
-  <si>
-    <t>Primary Phone</t>
-  </si>
-  <si>
-    <t>City, State</t>
-  </si>
-  <si>
-    <t>Child First Name</t>
-  </si>
-  <si>
-    <t>Child Last Name</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -140,30 +52,21 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -463,139 +366,297 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="X9" sqref="A2:X9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="10.33203125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="10"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="6.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="12.6640625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="13"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="9.5"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="14.83203125"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="14.5"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" width="10"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" width="5.83203125"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" width="10.1640625"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" width="9"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" width="13.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Primary Email</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Primary Phone</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>City, State</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Child First Name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Child Last Name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Email Date</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Response</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Response Date</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E2" s="2"/>
+    <row r="2">
+      <c r="E2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Antony</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Darsuma</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>codeninjas.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>icerain@uwalumni.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>3464123526</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Julius</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Darsuma</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Additional Information Child:Julius Darsuma Referrer:https://www.codeninjas.com/tx-cypress </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jes</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Byboth</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>codeninjas.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>jesbyboth@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>9794504780</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Aiden</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Byboth</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Additional Information Inquired About:Code Ninjas CREATE Program Slug:code-ninjas-create Child:Aiden Byboth Referrer:https://www.codeninjas.com/tx-cypress/code-ninjas-create/request-information </t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="14.5"/>
+    <col customWidth="1" max="2" min="2" width="17.1640625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="28.83203125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="26.1640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Template Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Subject</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Template Message</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Required Prompts</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="404" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
+    <row customHeight="1" ht="404" r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>[studentName], Join us at CodeNinjas!</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Hi [parentName], 
+This is Mike from CodeNinjas Cypress. Thank you for expressing interest in our program. Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something. I am sure that [studentName] will have a blast with one of our programs!
+Regards,
+CodeNinja Cypress</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[parentName],[studentName]</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+    <row customHeight="1" ht="409.5" r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Python Program</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>[studentName], Join us at CodeNinjas for our Python Program!</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>Hi [parentName], 
+This is Mike from CodeNinjas Cypress. Thank you for expressing interest in our program. Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something.Something something something something. I am sure that [studentName] will have a blast with one of our programs, especially our python program. We think it would be perfect for [studentName]
+Regards,
+CodeNinja Cypress</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[parentName],[studentName]</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>